<commit_message>
committing code to change the trial type after 10 correct trials
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/single_T_maze/Training_Trials _testing5.xlsx
+++ b/src/omniroute_operation/src/single_T_maze/Training_Trials _testing5.xlsx
@@ -194,11 +194,11 @@
   </sheetPr>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -238,11 +238,11 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.685531438809934</v>
+        <v>0.826877328749296</v>
       </c>
       <c r="F2" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.238302660350323</v>
+        <v>0.652206532753792</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,11 +260,11 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.144530583170006</v>
+        <v>0.3878575580271</v>
       </c>
       <c r="F3" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.376542643345598</v>
+        <v>0.320118588530593</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,11 +282,11 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.64572741481591</v>
+        <v>0.313243406266191</v>
       </c>
       <c r="F4" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.17399452323796</v>
+        <v>0.928471924551504</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,11 +304,11 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.903869240540268</v>
+        <v>0.91733703268575</v>
       </c>
       <c r="F5" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0420538453302305</v>
+        <v>0.682536005711955</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,11 +326,11 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.98214297657479</v>
+        <v>0.913175614688833</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.534024317640967</v>
+        <v>0.0546134835146121</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,11 +348,11 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.813488140464981</v>
+        <v>0.233184534744421</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0166192639506617</v>
+        <v>0.858891333823612</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,11 +370,11 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.267266095689758</v>
+        <v>0.914769587916589</v>
       </c>
       <c r="F8" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0757043724461236</v>
+        <v>0.83820944790251</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,11 +392,11 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.377680618334242</v>
+        <v>0.825574716103141</v>
       </c>
       <c r="F9" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.862597587257982</v>
+        <v>0.528648258385106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,11 +414,11 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.86480991412312</v>
+        <v>0.679577312207865</v>
       </c>
       <c r="F10" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.251723655984542</v>
+        <v>0.60743581491004</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,11 +436,11 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.45906629688552</v>
+        <v>0.614787276464844</v>
       </c>
       <c r="F11" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.369735804776497</v>
+        <v>0.0699886574841161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,11 +458,11 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.69184669125496</v>
+        <v>0.173800297149061</v>
       </c>
       <c r="F12" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.605330035508276</v>
+        <v>0.0811247724961397</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>10</v>
@@ -483,11 +483,11 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.410061279114616</v>
+        <v>0.746145403201307</v>
       </c>
       <c r="F13" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.427780289137538</v>
+        <v>0.826074655285237</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>10</v>
@@ -508,11 +508,11 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850433199174199</v>
+        <v>0.249224052200659</v>
       </c>
       <c r="F14" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.33067057911583</v>
+        <v>0.859341500040433</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>11</v>
@@ -533,11 +533,11 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.702035912184917</v>
+        <v>0.851492532436538</v>
       </c>
       <c r="F15" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.168962659967844</v>
+        <v>0.677434067569198</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>10</v>
@@ -558,11 +558,11 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.41536445077492</v>
+        <v>0.973825180037156</v>
       </c>
       <c r="F16" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.476770321120932</v>
+        <v>0.0534025399836561</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>11</v>
@@ -583,11 +583,11 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.882849724714859</v>
+        <v>0.733338834879582</v>
       </c>
       <c r="F17" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.849834415811843</v>
+        <v>0.546167640431614</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>10</v>
@@ -608,11 +608,11 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.433400215604287</v>
+        <v>0.549560522874322</v>
       </c>
       <c r="F18" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.127207221974192</v>
+        <v>0.0271678420048912</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>11</v>
@@ -633,11 +633,11 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.671244273267489</v>
+        <v>0.397985094517022</v>
       </c>
       <c r="F19" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.906332128601913</v>
+        <v>0.489148440813915</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>11</v>
@@ -658,11 +658,11 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.430312985545283</v>
+        <v>0.254288803787564</v>
       </c>
       <c r="F20" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210783143348885</v>
+        <v>0.159932189153179</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>10</v>
@@ -683,11 +683,11 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.473824022386394</v>
+        <v>0.517036191242262</v>
       </c>
       <c r="F21" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.136909179497688</v>
+        <v>0.199847152261879</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>11</v>
@@ -708,11 +708,11 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.563611313917925</v>
+        <v>0.865326690747754</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.090954885746548</v>
+        <v>0.214898192801335</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>10</v>
@@ -733,11 +733,11 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.65536000730306</v>
+        <v>0.581993365600963</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0340280253899847</v>
+        <v>0.191773023601629</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>11</v>
@@ -758,11 +758,11 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.798993536231935</v>
+        <v>0.414859512370313</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.364983392865821</v>
+        <v>0.084885815720278</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>10</v>
@@ -783,11 +783,11 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.848472875871312</v>
+        <v>0.381378163368496</v>
       </c>
       <c r="F25" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.472606990415131</v>
+        <v>0.166504281911293</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>10</v>
@@ -808,11 +808,11 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0782706848245193</v>
+        <v>0.309300057484778</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.769974934472731</v>
+        <v>0.111718144911302</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>11</v>
@@ -833,11 +833,11 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.673648546561175</v>
+        <v>0.828398165446914</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.374609533275918</v>
+        <v>0.00472819362898454</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>12</v>
@@ -858,11 +858,11 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.169423133178624</v>
+        <v>0.067735864373877</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.106325238305927</v>
+        <v>0.0959282739496349</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>12</v>
@@ -883,11 +883,11 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.536752765770121</v>
+        <v>0.397095115408509</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.19379745831896</v>
+        <v>0.161831739394636</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>12</v>
@@ -908,11 +908,11 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.944213919767126</v>
+        <v>0.616533601308234</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.226104079628807</v>
+        <v>0.306935286321051</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>13</v>
@@ -933,11 +933,11 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.904738911270954</v>
+        <v>0.732681531602834</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.654527575128777</v>
+        <v>0.958051447418227</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>13</v>
@@ -958,11 +958,11 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.993594408433868</v>
+        <v>0.579140097856992</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.426638193475488</v>
+        <v>0.46491978026832</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>12</v>
@@ -983,11 +983,11 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0717254207178719</v>
+        <v>0.608005174979176</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.173921906358908</v>
+        <v>0.235427625396809</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>13</v>
@@ -1008,11 +1008,11 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.946000607536833</v>
+        <v>0.526853731871459</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.665901777796011</v>
+        <v>0.497986318996932</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>12</v>
@@ -1033,11 +1033,11 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.858429165585568</v>
+        <v>0.691315129828268</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.18762917677837</v>
+        <v>0.61623858945345</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>13</v>
@@ -1058,11 +1058,11 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.619853372183679</v>
+        <v>0.442929446409727</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.37818520316657</v>
+        <v>0.205337485925469</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>12</v>
@@ -1083,11 +1083,11 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.940034892314794</v>
+        <v>0.0958008134404041</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.509746750381299</v>
+        <v>0.655257586858622</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>13</v>
@@ -1108,11 +1108,11 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.790245593959584</v>
+        <v>0.424976255895665</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.603975874980933</v>
+        <v>0.0344257545640207</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>13</v>
@@ -1133,11 +1133,11 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.988192302999901</v>
+        <v>0.12418358282316</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.472979714537621</v>
+        <v>0.283535889162879</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>13</v>
@@ -1158,11 +1158,11 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.468571377623125</v>
+        <v>0.342969945353559</v>
       </c>
       <c r="F40" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.559912729519084</v>
+        <v>0.943217623532069</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>12</v>
@@ -1183,11 +1183,11 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.219283101407545</v>
+        <v>0.703563210788746</v>
       </c>
       <c r="F41" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.249799044243456</v>
+        <v>0.918299782119238</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>13</v>
@@ -1201,18 +1201,18 @@
         <v>6</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.484685705048517</v>
+        <v>0.733913336658049</v>
       </c>
       <c r="F42" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.903016090067264</v>
+        <v>0.566065876555736</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>10</v>
@@ -1226,18 +1226,18 @@
         <v>6</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.805300033489346</v>
+        <v>0.0312321623246516</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.179106463991943</v>
+        <v>0.0868338850060116</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>12</v>
@@ -1251,18 +1251,18 @@
         <v>6</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0469254357931317</v>
+        <v>0.197747783415449</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.709532970372738</v>
+        <v>0.772746849439018</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>12</v>
@@ -1276,18 +1276,18 @@
         <v>6</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.43916879802868</v>
+        <v>0.12556098147061</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.567198601591221</v>
+        <v>0.149513789596399</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>12</v>
@@ -1301,18 +1301,18 @@
         <v>6</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.985370510912201</v>
+        <v>0.34679006388817</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.600798294098491</v>
+        <v>0.155621537990327</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>12</v>
@@ -1326,18 +1326,18 @@
         <v>7</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.929920720710372</v>
+        <v>0.18035786400503</v>
       </c>
       <c r="F47" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0690269038890247</v>
+        <v>0.0378925399804514</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>10</v>
@@ -1351,18 +1351,18 @@
         <v>7</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.400662242802532</v>
+        <v>0.697497047888929</v>
       </c>
       <c r="F48" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.732068460938405</v>
+        <v>0.114825829081349</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>12</v>
@@ -1376,18 +1376,18 @@
         <v>7</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.8057499077807</v>
+        <v>0.546630329924967</v>
       </c>
       <c r="F49" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.604100325793377</v>
+        <v>0.844472148104915</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>11</v>
@@ -1401,18 +1401,18 @@
         <v>7</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.716387897125024</v>
+        <v>0.736137484189733</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.229778083143192</v>
+        <v>0.914489004282059</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>13</v>
@@ -1426,18 +1426,18 @@
         <v>6</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.694448548864802</v>
+        <v>0.569300373510327</v>
       </c>
       <c r="F51" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.163724281757542</v>
+        <v>0.665157232907304</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>10</v>
@@ -1451,18 +1451,18 @@
         <v>6</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.37781322047164</v>
+        <v>0.260610154910675</v>
       </c>
       <c r="F52" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.411437289768202</v>
+        <v>0.208376063401212</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>12</v>
@@ -1483,11 +1483,11 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.666653006542377</v>
+        <v>0.836439924920689</v>
       </c>
       <c r="F53" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.483647043432646</v>
+        <v>0.993437593652203</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>10</v>
@@ -1508,11 +1508,11 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.362302553330031</v>
+        <v>0.606795084724289</v>
       </c>
       <c r="F54" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.584546563312112</v>
+        <v>0.768808763238962</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>10</v>
@@ -1533,11 +1533,11 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.492507220624615</v>
+        <v>0.266233167990823</v>
       </c>
       <c r="F55" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.230441075577122</v>
+        <v>0.897857624058103</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>12</v>
@@ -1558,11 +1558,11 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.824177106017313</v>
+        <v>0.443376785141018</v>
       </c>
       <c r="F56" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.700413435043977</v>
+        <v>0.93040824686754</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>10</v>
@@ -1583,11 +1583,11 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.624124041372594</v>
+        <v>0.598690274044303</v>
       </c>
       <c r="F57" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.899130997608377</v>
+        <v>0.433285667655012</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>13</v>
@@ -1608,11 +1608,11 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.239530260144416</v>
+        <v>0.14364785032777</v>
       </c>
       <c r="F58" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.98325517335959</v>
+        <v>0.82780664909057</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>11</v>
@@ -1633,11 +1633,11 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.578608664800121</v>
+        <v>0.0322518686227628</v>
       </c>
       <c r="F59" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.428804787980609</v>
+        <v>0.43075851369636</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>13</v>
@@ -1658,11 +1658,11 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.76807689992629</v>
+        <v>0.740841936432029</v>
       </c>
       <c r="F60" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0551325877807786</v>
+        <v>0.746924915065216</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>12</v>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.959824374442366</v>
+        <v>0.459016686863909</v>
       </c>
       <c r="F61" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.858469920428445</v>
+        <v>0.0616728556457535</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>13</v>

</xml_diff>